<commit_message>
Version 2.0 Terminada con calibracion
</commit_message>
<xml_diff>
--- a/Medidas/mediciones_voluntarios.xlsx
+++ b/Medidas/mediciones_voluntarios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,12 +470,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>pRUEBA 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-09-29_19-58-33</t>
+          <t>2025-09-29_20-53-09</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -496,243 +496,104 @@
     </row>
     <row r="3">
       <c r="D3" t="n">
-        <v>0.86</v>
+        <v>4.72</v>
       </c>
       <c r="E3" t="n">
-        <v>84.56</v>
+        <v>463.25</v>
       </c>
     </row>
     <row r="4">
       <c r="D4" t="n">
-        <v>0.9399999999999999</v>
+        <v>4.49</v>
       </c>
       <c r="E4" t="n">
-        <v>92.62</v>
+        <v>440.07</v>
       </c>
     </row>
     <row r="5">
       <c r="D5" t="n">
-        <v>1.03</v>
+        <v>4.01</v>
       </c>
       <c r="E5" t="n">
-        <v>100.65</v>
+        <v>393.71</v>
       </c>
     </row>
     <row r="6">
       <c r="D6" t="n">
-        <v>1.11</v>
+        <v>4.96</v>
       </c>
       <c r="E6" t="n">
-        <v>108.71</v>
+        <v>486.43</v>
       </c>
     </row>
     <row r="7">
       <c r="D7" t="n">
-        <v>1.07</v>
+        <v>4.72</v>
       </c>
       <c r="E7" t="n">
-        <v>104.68</v>
+        <v>463.25</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2025-09-29_20-00-02</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Epicóndilo lateral</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>MEDIDAS(Kgf/cm2)</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>MEDIDAS (kPa)</t>
-        </is>
+      <c r="D8" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="E8" t="n">
+        <v>486.43</v>
       </c>
     </row>
     <row r="9">
       <c r="D9" t="n">
-        <v>1</v>
+        <v>4.49</v>
       </c>
       <c r="E9" t="n">
-        <v>98.08</v>
+        <v>440.07</v>
       </c>
     </row>
     <row r="10">
-      <c r="D10" t="n">
-        <v>1.07</v>
-      </c>
-      <c r="E10" t="n">
-        <v>104.62</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Prueba 2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-09-29_20-54-16</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>MEDIDAS(Kgf/cm2)</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>MEDIDAS (kPa)</t>
+        </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>aa</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2025-09-29_20-04-49</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Epicóndilo lateral</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>MEDIDAS(Kgf/cm2)</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>MEDIDAS (kPa)</t>
-        </is>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>196.16</v>
       </c>
     </row>
     <row r="12">
       <c r="D12" t="n">
-        <v>2.29</v>
+        <v>1.88</v>
       </c>
       <c r="E12" t="n">
-        <v>224.19</v>
+        <v>183.89</v>
       </c>
     </row>
     <row r="13">
       <c r="D13" t="n">
-        <v>2.29</v>
+        <v>2.25</v>
       </c>
       <c r="E13" t="n">
-        <v>224.19</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="D14" t="n">
-        <v>2.86</v>
-      </c>
-      <c r="E14" t="n">
-        <v>280.29</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="D15" t="n">
-        <v>3.43</v>
-      </c>
-      <c r="E15" t="n">
-        <v>336.39</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="D16" t="n">
-        <v>3.14</v>
-      </c>
-      <c r="E16" t="n">
-        <v>308.34</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="D17" t="n">
-        <v>2.86</v>
-      </c>
-      <c r="E17" t="n">
-        <v>280.29</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="D19" t="n">
-        <v>2.29</v>
-      </c>
-      <c r="E19" t="n">
-        <v>224.19</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="D20" t="n">
-        <v>1.71</v>
-      </c>
-      <c r="E20" t="n">
-        <v>168.09</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="D21" t="n">
-        <v>2.29</v>
-      </c>
-      <c r="E21" t="n">
-        <v>224.19</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="D22" t="n">
-        <v>2.86</v>
-      </c>
-      <c r="E22" t="n">
-        <v>280.29</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2025-09-29_20-07-46</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Epicóndilo lateral</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>MEDIDAS(Kgf/cm2)</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>MEDIDAS (kPa)</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="D24" t="n">
-        <v>1.18</v>
-      </c>
-      <c r="E24" t="n">
-        <v>115.72</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="D25" t="n">
-        <v>2.36</v>
-      </c>
-      <c r="E25" t="n">
-        <v>231.62</v>
+        <v>220.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>